<commit_message>
Remove VSCode settings, update execution counts in Jupyter notebook, adjust Python version requirement, and add README with execution instructions.
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc2fde87aaa2ea9c/Python/Playwright_Scraping/.vscode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc2fde87aaa2ea9c/Python/Playwright_Scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3E0D1CAFA0DAD715E3088B352998CFB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C0C0A83-0EBA-41D2-A1DE-F9798B90EACC}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_0061D1A4D3F0D77BF7B82811595ED87656CDEF7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FA71E62-000B-40DC-8D61-6A613DAB32CF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
   <si>
     <t>productId</t>
   </si>
@@ -41,6 +41,186 @@
   </si>
   <si>
     <t>similarity_ratio</t>
+  </si>
+  <si>
+    <t>Mixer Daily Philips Walita - RI2530 - Branco</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07PW9QGTG</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07RQ9RGPS</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CX1TKC62</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0BRL9B8CW</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08DG13T6M</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B087442VX2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08749R2LT</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0874G5TTM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0874C3LHC</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08749DNHY</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0BVSDXMQJ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0874GFHT1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08YHR9C4S</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DCKBMVH9</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B09B2M8N4T</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CFM6RMLM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CFM67MPS</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B091V73RF5</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CZLXP9WS</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B097KP1641</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DT4VXWTX</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DTS94M48</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B076X7RQFQ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B076X76XW3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CWPKYCNM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DCPWN2FG</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CWPL7P17</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08BG687L9</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07SD5K7LR</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B09B2LVRCY</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B09TWPNFZX</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B076J168B8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B09N576NSY</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07574M6MR</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CFM7XGTQ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07SB1G4YJ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DP4YZS7R</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0C5S6137P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B097KPB52F</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CZMDPNK8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DP4X85Z3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CFM7757G</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07Z9SMB5F</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DFZJVTN6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CKG8898L</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0F1K3TV1P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0F1K49W28</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0F1K62YMQ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B09SVQVN77</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07735DD6K</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0F1K87VNG</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0F1K413NK</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B08QYRLPG1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CDJMQZ73</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B07K7YCMK5</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0765CWX6D</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0CXRJPWN9</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DL6CZ6XB</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/dp/B0DTXPM1NQ</t>
   </si>
 </sst>
 </file>
@@ -403,16 +583,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,6 +622,1386 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>229.9</v>
+      </c>
+      <c r="F2">
+        <v>134.91999999999999</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>314</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>229.9</v>
+      </c>
+      <c r="F3">
+        <v>136.72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>229.9</v>
+      </c>
+      <c r="F4">
+        <v>186.15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>314</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>229.9</v>
+      </c>
+      <c r="F5">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>314</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>229.9</v>
+      </c>
+      <c r="F6">
+        <v>169</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>229.9</v>
+      </c>
+      <c r="F7">
+        <v>257.25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>314</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>229.9</v>
+      </c>
+      <c r="F8">
+        <v>340.37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>314</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>229.9</v>
+      </c>
+      <c r="F9">
+        <v>260</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>314</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>229.9</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>314</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>229.9</v>
+      </c>
+      <c r="F11">
+        <v>220</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>314</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>229.9</v>
+      </c>
+      <c r="F12">
+        <v>147.9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>314</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>229.9</v>
+      </c>
+      <c r="F13">
+        <v>293.33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>314</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>229.9</v>
+      </c>
+      <c r="F14">
+        <v>185.89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>314</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>229.9</v>
+      </c>
+      <c r="F15">
+        <v>149.9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>314</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>229.9</v>
+      </c>
+      <c r="F16">
+        <v>189</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>314</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>229.9</v>
+      </c>
+      <c r="F17">
+        <v>220.92</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>314</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>229.9</v>
+      </c>
+      <c r="F18">
+        <v>220.92</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>314</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>229.9</v>
+      </c>
+      <c r="F19">
+        <v>68.98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>314</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>229.9</v>
+      </c>
+      <c r="F20">
+        <v>149</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>314</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>229.9</v>
+      </c>
+      <c r="F21">
+        <v>86.62</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>314</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>229.9</v>
+      </c>
+      <c r="F22">
+        <v>244.9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>314</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>229.9</v>
+      </c>
+      <c r="F23">
+        <v>20.9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>314</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>229.9</v>
+      </c>
+      <c r="F24">
+        <v>207</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>314</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>229.9</v>
+      </c>
+      <c r="F25">
+        <v>269.89999999999998</v>
+      </c>
+      <c r="G25" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>314</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>229.9</v>
+      </c>
+      <c r="F26">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>314</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>229.9</v>
+      </c>
+      <c r="F27">
+        <v>259.89999999999998</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>314</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>229.9</v>
+      </c>
+      <c r="F28">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>314</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>229.9</v>
+      </c>
+      <c r="F29">
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>314</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>229.9</v>
+      </c>
+      <c r="F30">
+        <v>200.52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>314</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>229.9</v>
+      </c>
+      <c r="F31">
+        <v>259</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>314</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>229.9</v>
+      </c>
+      <c r="F32">
+        <v>93.9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>314</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>229.9</v>
+      </c>
+      <c r="F33">
+        <v>149</v>
+      </c>
+      <c r="G33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>314</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>229.9</v>
+      </c>
+      <c r="F34">
+        <v>91.1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>314</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>229.9</v>
+      </c>
+      <c r="F35">
+        <v>227</v>
+      </c>
+      <c r="G35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>314</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>229.9</v>
+      </c>
+      <c r="F36">
+        <v>219.99</v>
+      </c>
+      <c r="G36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>314</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>229.9</v>
+      </c>
+      <c r="F37">
+        <v>128.25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>314</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>229.9</v>
+      </c>
+      <c r="F38">
+        <v>254.99</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>314</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>229.9</v>
+      </c>
+      <c r="F39">
+        <v>184.97</v>
+      </c>
+      <c r="G39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>314</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>229.9</v>
+      </c>
+      <c r="F40">
+        <v>152.62</v>
+      </c>
+      <c r="G40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>314</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>229.9</v>
+      </c>
+      <c r="F41">
+        <v>291.61</v>
+      </c>
+      <c r="G41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>314</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>229.9</v>
+      </c>
+      <c r="F42">
+        <v>239.99</v>
+      </c>
+      <c r="G42" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>314</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>229.9</v>
+      </c>
+      <c r="F43">
+        <v>180.41</v>
+      </c>
+      <c r="G43" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>314</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>229.9</v>
+      </c>
+      <c r="F44">
+        <v>105</v>
+      </c>
+      <c r="G44" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>314</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>229.9</v>
+      </c>
+      <c r="F45">
+        <v>55.9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>314</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>229.9</v>
+      </c>
+      <c r="F46">
+        <v>24</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>314</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>229.9</v>
+      </c>
+      <c r="F47">
+        <v>54.54</v>
+      </c>
+      <c r="G47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>314</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>229.9</v>
+      </c>
+      <c r="F48">
+        <v>59.99</v>
+      </c>
+      <c r="G48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H48">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>314</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>229.9</v>
+      </c>
+      <c r="F49">
+        <v>54.54</v>
+      </c>
+      <c r="G49" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>314</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>229.9</v>
+      </c>
+      <c r="F50">
+        <v>446.9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>56</v>
+      </c>
+      <c r="H50">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>314</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>229.9</v>
+      </c>
+      <c r="F51">
+        <v>129.9</v>
+      </c>
+      <c r="G51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H51">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>314</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>229.9</v>
+      </c>
+      <c r="F52">
+        <v>54.54</v>
+      </c>
+      <c r="G52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H52">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>314</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>229.9</v>
+      </c>
+      <c r="F53">
+        <v>72.72</v>
+      </c>
+      <c r="G53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>314</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>229.9</v>
+      </c>
+      <c r="F54">
+        <v>473.37</v>
+      </c>
+      <c r="G54" t="s">
+        <v>60</v>
+      </c>
+      <c r="H54">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>314</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>229.9</v>
+      </c>
+      <c r="F55">
+        <v>629.9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>314</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>229.9</v>
+      </c>
+      <c r="F56">
+        <v>319.89999999999998</v>
+      </c>
+      <c r="G56" t="s">
+        <v>62</v>
+      </c>
+      <c r="H56">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>314</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>229.9</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>63</v>
+      </c>
+      <c r="H57">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>314</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58">
+        <v>229.9</v>
+      </c>
+      <c r="F58">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="G58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H58">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>314</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <v>229.9</v>
+      </c>
+      <c r="F59">
+        <v>195.3</v>
+      </c>
+      <c r="G59" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>314</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>229.9</v>
+      </c>
+      <c r="F60">
+        <v>108.79</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60">
+        <v>4.1666666666666012E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>314</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>229.9</v>
+      </c>
+      <c r="F61">
+        <v>20.9</v>
+      </c>
+      <c r="G61" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61">
+        <v>4.1666666666666012E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>